<commit_message>
adding an algorithm for selecting questions in case of the last lack, work in process
</commit_message>
<xml_diff>
--- a/Test Data.xlsx
+++ b/Test Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4206669-9D40-4247-8C94-0ECD7E1B31E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86870BAF-E167-4CCB-9C00-2F2715F02EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" xr2:uid="{912DC69B-E7B6-4014-ADA9-E64C2D74106E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="89">
   <si>
     <t>All questions</t>
   </si>
@@ -72,21 +72,12 @@
     <t>QU</t>
   </si>
   <si>
-    <t>[10, QUt-1]</t>
-  </si>
-  <si>
     <t>QUt</t>
   </si>
   <si>
     <t>the same tests as 26-61, but QP instead QU in Length</t>
   </si>
   <si>
-    <t>[10, 200]</t>
-  </si>
-  <si>
-    <t>[5, QU-1]</t>
-  </si>
-  <si>
     <t>[QU+1, QP-1]</t>
   </si>
   <si>
@@ -96,24 +87,15 @@
     <t>the same tests as 56-61</t>
   </si>
   <si>
-    <t>[10, QU-1]</t>
-  </si>
-  <si>
     <t>the same tests as 26-61</t>
   </si>
   <si>
-    <t>[5, QP-1]</t>
-  </si>
-  <si>
     <t>[QP+1, QU-1]</t>
   </si>
   <si>
     <t>[QU+1, 202]</t>
   </si>
   <si>
-    <t>[10, QP-1]</t>
-  </si>
-  <si>
     <t>[QUt+1, 5000]</t>
   </si>
   <si>
@@ -123,9 +105,6 @@
     <t>QN</t>
   </si>
   <si>
-    <t>[3, QU-1]</t>
-  </si>
-  <si>
     <t>[QP+1, SUM(QP+QU)-1]</t>
   </si>
   <si>
@@ -159,9 +138,6 @@
     <t>the same tests as 63-76, but QP instead of QU, and QN instead of QP in Length</t>
   </si>
   <si>
-    <t>[20, 200]</t>
-  </si>
-  <si>
     <t>SUM(QU+QP)</t>
   </si>
   <si>
@@ -180,9 +156,6 @@
     <t>[SUM(QN+QU)+1, SUM(QN+QP+QU)-1]</t>
   </si>
   <si>
-    <t>[10, 50]</t>
-  </si>
-  <si>
     <t>[60, 100]</t>
   </si>
   <si>
@@ -310,6 +283,21 @@
   </si>
   <si>
     <t>1 "120"</t>
+  </si>
+  <si>
+    <t>[40, 200]</t>
+  </si>
+  <si>
+    <t>[40, 50]</t>
+  </si>
+  <si>
+    <t>[30, QU-1]</t>
+  </si>
+  <si>
+    <t>[30, QUt-1]</t>
+  </si>
+  <si>
+    <t>[30, QP-1]</t>
   </si>
 </sst>
 </file>
@@ -842,8 +830,8 @@
   <dimension ref="A1:I198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A198" sqref="A198"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +861,7 @@
       </c>
       <c r="G1" s="12"/>
       <c r="I1" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1409,13 +1397,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1432,13 +1420,13 @@
         <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1455,13 +1443,13 @@
         <v>0</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1478,13 +1466,13 @@
         <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>9</v>
@@ -1501,13 +1489,13 @@
         <v>0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>9</v>
@@ -1524,13 +1512,13 @@
         <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -1547,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>5</v>
@@ -1570,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>5</v>
@@ -1593,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>5</v>
@@ -1616,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -1639,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
@@ -1662,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>5</v>
@@ -1685,13 +1673,13 @@
         <v>0</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -1708,13 +1696,13 @@
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
@@ -1731,13 +1719,13 @@
         <v>0</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
@@ -1754,13 +1742,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>9</v>
@@ -1777,13 +1765,13 @@
         <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>9</v>
@@ -1800,13 +1788,13 @@
         <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
@@ -1823,13 +1811,13 @@
         <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="F44" s="1">
         <v>0</v>
@@ -1846,13 +1834,13 @@
         <v>0</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
@@ -1869,13 +1857,13 @@
         <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -1892,13 +1880,13 @@
         <v>0</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>9</v>
@@ -1915,13 +1903,13 @@
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>9</v>
@@ -1938,13 +1926,13 @@
         <v>0</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
@@ -1961,13 +1949,13 @@
         <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
@@ -1984,13 +1972,13 @@
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -2007,13 +1995,13 @@
         <v>0</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -2030,13 +2018,13 @@
         <v>0</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>9</v>
@@ -2053,13 +2041,13 @@
         <v>0</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>9</v>
@@ -2076,13 +2064,13 @@
         <v>0</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -2099,13 +2087,13 @@
         <v>0</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -2122,13 +2110,13 @@
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -2145,13 +2133,13 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F58" s="1">
         <v>0</v>
@@ -2168,13 +2156,13 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>9</v>
@@ -2191,13 +2179,13 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>9</v>
@@ -2214,13 +2202,13 @@
         <v>0</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F61" s="1">
         <v>1</v>
@@ -2234,13 +2222,13 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="C62" s="1">
         <v>0</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2248,19 +2236,19 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2268,10 +2256,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>5</v>
@@ -2280,7 +2268,7 @@
         <v>12</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2288,19 +2276,19 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2308,19 +2296,19 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2328,19 +2316,19 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,19 +2336,19 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2368,19 +2356,19 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2388,19 +2376,19 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2408,10 +2396,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>8</v>
@@ -2420,7 +2408,7 @@
         <v>12</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2428,19 +2416,19 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2448,19 +2436,19 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2468,19 +2456,19 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2488,19 +2476,19 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,19 +2496,19 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2528,13 +2516,13 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D77" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2542,13 +2530,13 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D78" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2556,13 +2544,13 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D79" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2570,19 +2558,19 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2590,19 +2578,19 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2610,19 +2598,19 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2630,10 +2618,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>5</v>
@@ -2642,7 +2630,7 @@
         <v>12</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2650,19 +2638,19 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2670,19 +2658,19 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2690,19 +2678,19 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2710,19 +2698,19 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2730,19 +2718,19 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2750,19 +2738,19 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2770,10 +2758,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>8</v>
@@ -2782,7 +2770,7 @@
         <v>12</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2790,19 +2778,19 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2810,19 +2798,19 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2830,24 +2818,24 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="B94" s="1">
         <v>0</v>
@@ -2856,867 +2844,867 @@
         <v>0</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B95" s="1">
         <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B96" s="1">
         <v>0</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B97" s="1">
         <v>0</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C146" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E146" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -3727,20 +3715,20 @@
         <v>0</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E148" s="10">
         <v>5</v>
       </c>
       <c r="F148" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G148" s="10"/>
       <c r="I148" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -3751,20 +3739,20 @@
         <v>0</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D149" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E149" s="10">
         <v>5</v>
       </c>
       <c r="F149" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G149" s="10"/>
       <c r="I149" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -3775,20 +3763,20 @@
         <v>0</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D150" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E150" s="10">
         <v>50</v>
       </c>
       <c r="F150" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G150" s="10"/>
       <c r="I150" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -3799,20 +3787,20 @@
         <v>0</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D151" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E151" s="10">
         <v>100</v>
       </c>
       <c r="F151" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G151" s="10"/>
       <c r="I151" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -3820,23 +3808,23 @@
         <v>0</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C152" s="10">
         <v>0</v>
       </c>
       <c r="D152" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E152" s="10">
         <v>5</v>
       </c>
       <c r="F152" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G152" s="10"/>
       <c r="I152" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -3844,23 +3832,23 @@
         <v>0</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C153" s="10">
         <v>0</v>
       </c>
       <c r="D153" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E153" s="10">
         <v>5</v>
       </c>
       <c r="F153" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G153" s="10"/>
       <c r="I153" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -3868,23 +3856,23 @@
         <v>0</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C154" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D154" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E154" s="10">
         <v>5</v>
       </c>
       <c r="F154" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G154" s="10"/>
       <c r="I154" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -3892,23 +3880,23 @@
         <v>0</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D155" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E155" s="10">
         <v>5</v>
       </c>
       <c r="F155" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G155" s="10"/>
       <c r="I155" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -3916,23 +3904,23 @@
         <v>0</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C156" s="10">
         <v>0</v>
       </c>
       <c r="D156" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E156" s="10">
         <v>50</v>
       </c>
       <c r="F156" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G156" s="10"/>
       <c r="I156" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -3940,23 +3928,23 @@
         <v>0</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D157" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E157" s="10">
         <v>50</v>
       </c>
       <c r="F157" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G157" s="10"/>
       <c r="I157" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -3964,23 +3952,23 @@
         <v>0</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D158" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E158" s="10">
         <v>50</v>
       </c>
       <c r="F158" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G158" s="10"/>
       <c r="I158" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -3988,23 +3976,23 @@
         <v>0</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C159" s="10">
         <v>0</v>
       </c>
       <c r="D159" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E159" s="10">
         <v>100</v>
       </c>
       <c r="F159" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G159" s="10"/>
       <c r="I159" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -4012,23 +4000,23 @@
         <v>0</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C160" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D160" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E160" s="10">
         <v>100</v>
       </c>
       <c r="F160" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G160" s="10"/>
       <c r="I160" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -4036,23 +4024,23 @@
         <v>0</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D161" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E161" s="10">
         <v>100</v>
       </c>
       <c r="F161" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G161" s="10"/>
       <c r="I161" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -4060,23 +4048,23 @@
         <v>0</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D162" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E162" s="10">
         <v>100</v>
       </c>
       <c r="F162" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G162" s="10"/>
       <c r="I162" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -4084,28 +4072,28 @@
         <v>0</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D163" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E163" s="10">
         <v>100</v>
       </c>
       <c r="F163" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G163" s="10"/>
       <c r="I163" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B164" s="10">
         <v>0</v>
@@ -4114,22 +4102,22 @@
         <v>0</v>
       </c>
       <c r="D164" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E164" s="10">
         <v>5</v>
       </c>
       <c r="F164" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G164" s="10"/>
       <c r="I164" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B165" s="10">
         <v>0</v>
@@ -4138,190 +4126,190 @@
         <v>0</v>
       </c>
       <c r="D165" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E165" s="10">
         <v>5</v>
       </c>
       <c r="F165" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G165" s="10"/>
       <c r="I165" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B166" s="10">
         <v>0</v>
       </c>
       <c r="C166" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D166" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E166" s="10">
         <v>5</v>
       </c>
       <c r="F166" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G166" s="10"/>
       <c r="I166" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B167" s="10">
         <v>0</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D167" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E167" s="10">
         <v>5</v>
       </c>
       <c r="F167" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G167" s="10"/>
       <c r="I167" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B168" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C168" s="10">
         <v>0</v>
       </c>
       <c r="D168" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E168" s="10">
         <v>5</v>
       </c>
       <c r="F168" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G168" s="10"/>
       <c r="I168" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C169" s="10">
         <v>0</v>
       </c>
       <c r="D169" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E169" s="10">
         <v>5</v>
       </c>
       <c r="F169" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G169" s="10"/>
       <c r="I169" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B170" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D170" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E170" s="10">
         <v>5</v>
       </c>
       <c r="F170" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G170" s="10"/>
       <c r="I170" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D171" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E171" s="10">
         <v>5</v>
       </c>
       <c r="F171" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G171" s="10"/>
       <c r="I171" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C172" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E172" s="10">
         <v>5</v>
       </c>
       <c r="F172" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G172" s="10"/>
       <c r="I172" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="10" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B173" s="10">
         <v>0</v>
@@ -4330,190 +4318,190 @@
         <v>0</v>
       </c>
       <c r="D173" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E173" s="10">
         <v>50</v>
       </c>
       <c r="F173" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G173" s="10"/>
       <c r="I173" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B174" s="10">
         <v>0</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D174" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E174" s="10">
         <v>50</v>
       </c>
       <c r="F174" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G174" s="10"/>
       <c r="I174" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B175" s="10">
         <v>0</v>
       </c>
       <c r="C175" s="10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E175" s="10">
         <v>50</v>
       </c>
       <c r="F175" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G175" s="10"/>
       <c r="I175" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B176" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C176" s="10">
         <v>0</v>
       </c>
       <c r="D176" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E176" s="10">
         <v>50</v>
       </c>
       <c r="F176" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G176" s="10"/>
       <c r="I176" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C177" s="10">
         <v>0</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E177" s="10">
         <v>50</v>
       </c>
       <c r="F177" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G177" s="10"/>
       <c r="I177" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B178" s="10" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C178" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E178" s="10">
         <v>50</v>
       </c>
       <c r="F178" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G178" s="10"/>
       <c r="I178" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C179" s="10" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D179" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E179" s="10">
         <v>50</v>
       </c>
       <c r="F179" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G179" s="10"/>
       <c r="I179" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B180" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B180" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="C180" s="10" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E180" s="10">
         <v>50</v>
       </c>
       <c r="F180" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G180" s="10"/>
       <c r="I180" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B181" s="10">
         <v>0</v>
@@ -4522,425 +4510,425 @@
         <v>0</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E181" s="10">
         <v>100</v>
       </c>
       <c r="F181" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G181" s="10"/>
       <c r="I181" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B182" s="10">
         <v>0</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D182" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E182" s="10">
         <v>100</v>
       </c>
       <c r="F182" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G182" s="10"/>
       <c r="I182" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B183" s="10">
         <v>0</v>
       </c>
       <c r="C183" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E183" s="10">
         <v>100</v>
       </c>
       <c r="F183" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G183" s="10"/>
       <c r="I183" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B184" s="10">
         <v>0</v>
       </c>
       <c r="C184" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D184" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E184" s="10">
         <v>100</v>
       </c>
       <c r="F184" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G184" s="10"/>
       <c r="I184" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B185" s="10">
         <v>0</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D185" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E185" s="10">
         <v>100</v>
       </c>
       <c r="F185" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G185" s="10"/>
       <c r="I185" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C186" s="10">
         <v>0</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E186" s="10">
         <v>100</v>
       </c>
       <c r="F186" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G186" s="10"/>
       <c r="I186" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C187" s="10">
         <v>0</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E187" s="10">
         <v>100</v>
       </c>
       <c r="F187" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G187" s="10"/>
       <c r="I187" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B188" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C188" s="10">
         <v>0</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E188" s="10">
         <v>100</v>
       </c>
       <c r="F188" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G188" s="10"/>
       <c r="I188" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C189" s="10">
         <v>0</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E189" s="10">
         <v>100</v>
       </c>
       <c r="F189" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G189" s="10"/>
       <c r="I189" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="10" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B190" s="10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C190" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E190" s="10">
         <v>100</v>
       </c>
       <c r="F190" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G190" s="10"/>
       <c r="I190" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B191" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E191" s="10">
         <v>100</v>
       </c>
       <c r="F191" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G191" s="10"/>
       <c r="I191" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B192" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C192" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D192" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E192" s="10">
         <v>100</v>
       </c>
       <c r="F192" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G192" s="10"/>
       <c r="I192" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B193" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C193" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D193" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E193" s="10">
         <v>100</v>
       </c>
       <c r="F193" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G193" s="10"/>
       <c r="I193" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B194" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C194" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E194" s="10">
         <v>100</v>
       </c>
       <c r="F194" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G194" s="10"/>
       <c r="I194" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B195" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C195" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D195" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E195" s="10">
         <v>100</v>
       </c>
       <c r="F195" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G195" s="10"/>
       <c r="I195" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B196" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C196" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E196" s="10">
         <v>100</v>
       </c>
       <c r="F196" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G196" s="10"/>
       <c r="I196" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="10" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B197" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C197" s="10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D197" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E197" s="10">
         <v>100</v>
       </c>
       <c r="F197" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G197" s="10"/>
       <c r="I197" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B198" s="10" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C198" s="10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E198" s="10">
         <v>100</v>
       </c>
       <c r="F198" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G198" s="10"/>
       <c r="I198" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GetFullEstimatedTimeOfQuestion() was moved to Extensions, added unit tests for it
</commit_message>
<xml_diff>
--- a/Test Data.xlsx
+++ b/Test Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86870BAF-E167-4CCB-9C00-2F2715F02EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B46EF5-9779-4270-B1BF-FD3DBC14899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" xr2:uid="{912DC69B-E7B6-4014-ADA9-E64C2D74106E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="92">
   <si>
     <t>All questions</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>[30, QP-1]</t>
+  </si>
+  <si>
+    <t>1 "50"</t>
+  </si>
+  <si>
+    <t>1 "99"</t>
+  </si>
+  <si>
+    <t>"99"</t>
   </si>
 </sst>
 </file>
@@ -827,11 +836,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75537EE-2FD5-44C1-8F49-C84E9EBD454F}">
-  <dimension ref="A1:I198"/>
+  <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E138" sqref="E138"/>
+      <pane ySplit="2" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4931,6 +4940,30 @@
         <v>65</v>
       </c>
     </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B200" s="10">
+        <v>0</v>
+      </c>
+      <c r="C200" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D200" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E200" s="10">
+        <v>5</v>
+      </c>
+      <c r="F200" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G200" s="10"/>
+      <c r="I200" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
refreshed test data file
</commit_message>
<xml_diff>
--- a/Test Data.xlsx
+++ b/Test Data.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B46EF5-9779-4270-B1BF-FD3DBC14899A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B78A9D-6937-48F1-B350-78E78DF6819A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" xr2:uid="{912DC69B-E7B6-4014-ADA9-E64C2D74106E}"/>
+    <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{912DC69B-E7B6-4014-ADA9-E64C2D74106E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Data" sheetId="1" r:id="rId1"/>
+    <sheet name="SelectQuestionsForTraining" sheetId="1" r:id="rId1"/>
+    <sheet name="UpdateQuestionStatus" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="107">
   <si>
     <t>All questions</t>
   </si>
@@ -307,13 +308,58 @@
   </si>
   <si>
     <t>"99"</t>
+  </si>
+  <si>
+    <t>Exists?</t>
+  </si>
+  <si>
+    <t>IsNew?</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Correct answer?</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>&gt;50</t>
+  </si>
+  <si>
+    <t>[1,MAX-1]</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>aR-1</t>
+  </si>
+  <si>
+    <t>aP+1</t>
+  </si>
+  <si>
+    <t>aP-1</t>
+  </si>
+  <si>
+    <t>[2,49]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,8 +373,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,6 +399,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -492,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -522,6 +583,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,9 +923,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75537EE-2FD5-44C1-8F49-C84E9EBD454F}">
   <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A164" sqref="A164"/>
+      <selection pane="bottomLeft" activeCell="E216" sqref="E216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4975,4 +5060,1673 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC61AC4-7B41-4422-8DF2-C4F2A8FD33B8}">
+  <dimension ref="A1:H64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="2">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="1">
+        <v>49</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="1">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="1">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="1">
+        <v>50</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="1">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="1">
+        <v>50</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="1">
+        <v>50</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="1">
+        <v>50</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="1">
+        <v>50</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="1">
+        <v>50</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="1">
+        <v>50</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="1">
+        <v>50</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="1">
+        <v>50</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="1">
+        <v>50</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="1">
+        <v>50</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="1">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="1">
+        <v>50</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="1">
+        <v>50</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="1">
+        <v>50</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="24">
+        <v>0</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="24">
+        <v>50</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="24">
+        <v>0</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="24">
+        <v>50</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="24">
+        <v>50</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="24">
+        <v>0</v>
+      </c>
+      <c r="D35" s="24">
+        <v>0</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="24">
+        <v>0</v>
+      </c>
+      <c r="H35" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="24">
+        <v>0</v>
+      </c>
+      <c r="D36" s="24">
+        <v>0</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" s="24">
+        <v>50</v>
+      </c>
+      <c r="H36" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="24">
+        <v>0</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G37" s="24">
+        <v>0</v>
+      </c>
+      <c r="H37" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="24">
+        <v>0</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G38" s="24">
+        <v>50</v>
+      </c>
+      <c r="H38" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="24">
+        <v>0</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="24">
+        <v>0</v>
+      </c>
+      <c r="H39" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="24">
+        <v>0</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" s="24">
+        <v>50</v>
+      </c>
+      <c r="H40" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="24">
+        <v>1</v>
+      </c>
+      <c r="D41" s="24">
+        <v>0</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" s="24">
+        <v>1</v>
+      </c>
+      <c r="H41" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="24">
+        <v>1</v>
+      </c>
+      <c r="D42" s="24">
+        <v>0</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42" s="24">
+        <v>50</v>
+      </c>
+      <c r="H42" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="24">
+        <v>1</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G43" s="24">
+        <v>1</v>
+      </c>
+      <c r="H43" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="24">
+        <v>1</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G44" s="24">
+        <v>50</v>
+      </c>
+      <c r="H44" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="24">
+        <v>1</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G45" s="24">
+        <v>1</v>
+      </c>
+      <c r="H45" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="24">
+        <v>1</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G46" s="24">
+        <v>50</v>
+      </c>
+      <c r="H46" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="24">
+        <v>0</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="24">
+        <v>0</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G48" s="24">
+        <v>50</v>
+      </c>
+      <c r="H48" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G50" s="24">
+        <v>50</v>
+      </c>
+      <c r="H50" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H51" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G52" s="24">
+        <v>50</v>
+      </c>
+      <c r="H52" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="1">
+        <v>50</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="1">
+        <v>50</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G54" s="1">
+        <v>50</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="24">
+        <v>50</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F55" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G55" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="24">
+        <v>50</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G56" s="24">
+        <v>50</v>
+      </c>
+      <c r="H56" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="24">
+        <v>50</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G57" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H57" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="24">
+        <v>50</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F58" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G58" s="24">
+        <v>50</v>
+      </c>
+      <c r="H58" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" s="24">
+        <v>0</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G59" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H59" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D60" s="24">
+        <v>0</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F60" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G60" s="24">
+        <v>50</v>
+      </c>
+      <c r="H60" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G61" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H61" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G62" s="24">
+        <v>50</v>
+      </c>
+      <c r="H62" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G63" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="H63" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G64" s="24">
+        <v>50</v>
+      </c>
+      <c r="H64" s="24">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refreshed test data file for Algorithm
</commit_message>
<xml_diff>
--- a/Test Data.xlsx
+++ b/Test Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B78A9D-6937-48F1-B350-78E78DF6819A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52BE963-F3D7-4C76-B0E6-952F350D1425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5355" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{912DC69B-E7B6-4014-ADA9-E64C2D74106E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="107">
   <si>
     <t>All questions</t>
   </si>
@@ -334,9 +334,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>&gt;50</t>
-  </si>
-  <si>
     <t>[1,MAX-1]</t>
   </si>
   <si>
@@ -353,6 +350,9 @@
   </si>
   <si>
     <t>[2,49]</t>
+  </si>
+  <si>
+    <t>aR</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,12 +399,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -565,6 +559,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -589,24 +595,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,21 +930,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="15" t="s">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="12"/>
+      <c r="G1" s="16"/>
       <c r="I1" s="3" t="s">
         <v>58</v>
       </c>
@@ -968,8 +959,8 @@
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="14"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -5064,11 +5055,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC61AC4-7B41-4422-8DF2-C4F2A8FD33B8}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5083,43 +5074,43 @@
     <col min="8" max="8" width="5.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-    </row>
-    <row r="2" spans="1:8" s="23" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:8" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="13" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5183,7 +5174,7 @@
         <v>50</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5223,7 +5214,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>98</v>
@@ -5235,7 +5226,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5249,7 +5240,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>99</v>
@@ -5261,7 +5252,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5275,7 +5266,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>98</v>
@@ -5287,7 +5278,7 @@
         <v>50</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5301,7 +5292,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>99</v>
@@ -5313,7 +5304,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5339,7 +5330,7 @@
         <v>50</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5379,7 +5370,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>98</v>
@@ -5391,7 +5382,7 @@
         <v>50</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5405,7 +5396,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>99</v>
@@ -5417,7 +5408,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5431,7 +5422,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>98</v>
@@ -5443,7 +5434,7 @@
         <v>50</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5457,7 +5448,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>99</v>
@@ -5469,7 +5460,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5480,7 +5471,7 @@
         <v>98</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -5495,7 +5486,7 @@
         <v>50</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5506,7 +5497,7 @@
         <v>98</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -5518,7 +5509,7 @@
         <v>98</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -5532,10 +5523,10 @@
         <v>98</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>98</v>
@@ -5547,7 +5538,7 @@
         <v>50</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5558,10 +5549,10 @@
         <v>98</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>99</v>
@@ -5570,10 +5561,10 @@
         <v>98</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -5584,10 +5575,10 @@
         <v>98</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>98</v>
@@ -5599,7 +5590,7 @@
         <v>50</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5610,10 +5601,10 @@
         <v>98</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>99</v>
@@ -5622,10 +5613,10 @@
         <v>98</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5651,7 +5642,7 @@
         <v>50</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5674,7 +5665,7 @@
         <v>98</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
@@ -5691,7 +5682,7 @@
         <v>50</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>98</v>
@@ -5703,7 +5694,7 @@
         <v>50</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5717,7 +5708,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>99</v>
@@ -5726,10 +5717,10 @@
         <v>98</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -5743,7 +5734,7 @@
         <v>50</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>98</v>
@@ -5755,7 +5746,7 @@
         <v>50</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -5769,7 +5760,7 @@
         <v>50</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>99</v>
@@ -5778,945 +5769,61 @@
         <v>98</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="24">
-        <v>0</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G29" s="24">
+      <c r="B29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="1">
         <v>50</v>
       </c>
-      <c r="H29" s="24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="24">
-        <v>0</v>
-      </c>
-      <c r="E30" s="24" t="s">
+      <c r="F29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F30" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H30" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="B30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G31" s="24">
+      <c r="C30" s="1">
         <v>50</v>
       </c>
-      <c r="H31" s="24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G32" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H32" s="24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F33" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G33" s="24">
+      <c r="G30" s="1">
         <v>50</v>
       </c>
-      <c r="H33" s="24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G34" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H34" s="24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="24">
-        <v>0</v>
-      </c>
-      <c r="D35" s="24">
-        <v>0</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G35" s="24">
-        <v>0</v>
-      </c>
-      <c r="H35" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="24">
-        <v>0</v>
-      </c>
-      <c r="D36" s="24">
-        <v>0</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G36" s="24">
-        <v>50</v>
-      </c>
-      <c r="H36" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="24">
-        <v>0</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G37" s="24">
-        <v>0</v>
-      </c>
-      <c r="H37" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" s="24">
-        <v>0</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G38" s="24">
-        <v>50</v>
-      </c>
-      <c r="H38" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" s="24">
-        <v>0</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G39" s="24">
-        <v>0</v>
-      </c>
-      <c r="H39" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" s="24">
-        <v>0</v>
-      </c>
-      <c r="D40" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G40" s="24">
-        <v>50</v>
-      </c>
-      <c r="H40" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="24">
-        <v>1</v>
-      </c>
-      <c r="D41" s="24">
-        <v>0</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F41" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G41" s="24">
-        <v>1</v>
-      </c>
-      <c r="H41" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="24">
-        <v>1</v>
-      </c>
-      <c r="D42" s="24">
-        <v>0</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G42" s="24">
-        <v>50</v>
-      </c>
-      <c r="H42" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" s="24">
-        <v>1</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G43" s="24">
-        <v>1</v>
-      </c>
-      <c r="H43" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" s="24">
-        <v>1</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F44" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G44" s="24">
-        <v>50</v>
-      </c>
-      <c r="H44" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="24">
-        <v>1</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F45" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G45" s="24">
-        <v>1</v>
-      </c>
-      <c r="H45" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="24">
-        <v>1</v>
-      </c>
-      <c r="D46" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E46" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G46" s="24">
-        <v>50</v>
-      </c>
-      <c r="H46" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="24">
-        <v>0</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F47" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G47" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H47" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" s="24">
-        <v>0</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G48" s="24">
-        <v>50</v>
-      </c>
-      <c r="H48" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E49" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G49" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H49" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F50" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G50" s="24">
-        <v>50</v>
-      </c>
-      <c r="H50" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E51" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F51" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G51" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H51" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G52" s="24">
-        <v>50</v>
-      </c>
-      <c r="H52" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="1">
-        <v>50</v>
-      </c>
-      <c r="D53" s="1">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H53" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C54" s="1">
-        <v>50</v>
-      </c>
-      <c r="D54" s="1">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G54" s="1">
-        <v>50</v>
-      </c>
-      <c r="H54" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B55" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="24">
-        <v>50</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E55" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F55" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G55" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H55" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B56" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56" s="24">
-        <v>50</v>
-      </c>
-      <c r="D56" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G56" s="24">
-        <v>50</v>
-      </c>
-      <c r="H56" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C57" s="24">
-        <v>50</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E57" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F57" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G57" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H57" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B58" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58" s="24">
-        <v>50</v>
-      </c>
-      <c r="D58" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="F58" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G58" s="24">
-        <v>50</v>
-      </c>
-      <c r="H58" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B59" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="24">
-        <v>0</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F59" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G59" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H59" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D60" s="24">
-        <v>0</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F60" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G60" s="24">
-        <v>50</v>
-      </c>
-      <c r="H60" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B61" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F61" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G61" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H61" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B62" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D62" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F62" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G62" s="24">
-        <v>50</v>
-      </c>
-      <c r="H62" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B63" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G63" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="H63" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B64" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D64" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="G64" s="24">
-        <v>50</v>
-      </c>
-      <c r="H64" s="24">
+      <c r="H30" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>